<commit_message>
Mol raw col names uniformization
</commit_message>
<xml_diff>
--- a/Multi-taxa_data/MollEchino/Mol_raw/Mol_div_AW.xlsx
+++ b/Multi-taxa_data/MollEchino/Mol_raw/Mol_div_AW.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claud\Documents\COMUNE\STUDIO.LAVORO\IMBRSea\Thesis\StatAnalysis\Multi-taxa_data\MollEchino\Mol_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{595AE7DC-613F-4714-B96B-628BB6E6AFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDD6626-CDDA-45DA-A6B2-41AF61F4D120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,9 +62,6 @@
     <t>SPECIES</t>
   </si>
   <si>
-    <t>SIZE</t>
-  </si>
-  <si>
     <t>NOTES</t>
   </si>
   <si>
@@ -186,13 +183,16 @@
   </si>
   <si>
     <t>P5260063</t>
+  </si>
+  <si>
+    <t>SIZE (cm)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -216,6 +216,12 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -237,11 +243,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,15 +467,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -481,449 +488,450 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="2"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="B2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="K2" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="K3" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="F4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="K4" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="E5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K5" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="F6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="K6" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="E7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K7" s="3">
         <v>4.5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="E8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K8" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="E9" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="K9" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="E10" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="K10" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="E11" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K11" s="3">
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="E12" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K12" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="E13" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="J13" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="K13" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="E14" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="J14" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="K14" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="F15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J15" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="K15" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="F16" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K16" s="3">
         <v>2</v>
@@ -931,28 +939,28 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G17" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="J17" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K17" s="3">
         <v>5</v>
@@ -960,28 +968,28 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="J18" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="K18" s="3">
         <v>4</v>
@@ -989,28 +997,28 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K19" s="3">
         <v>1.5</v>
@@ -1018,28 +1026,28 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="J20" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="K20" s="3">
         <v>1</v>
@@ -1047,28 +1055,28 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="F21" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K21" s="3">
         <v>4</v>
@@ -1076,28 +1084,28 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K22" s="3">
         <v>3</v>
@@ -1105,28 +1113,28 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K23" s="3">
         <v>3</v>
@@ -1134,28 +1142,28 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K24" s="3">
         <v>5</v>
@@ -1163,28 +1171,28 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K25" s="3">
         <v>3</v>
@@ -1192,28 +1200,28 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K26" s="3">
         <v>1</v>
@@ -1221,28 +1229,28 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="J27" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="K27" s="3">
         <v>1.5</v>
@@ -1250,28 +1258,28 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K28" s="3">
         <v>3.5</v>
@@ -1279,28 +1287,28 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="F29" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K29" s="3">
         <v>4</v>
@@ -1308,28 +1316,28 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K30" s="3">
         <v>2.5</v>
@@ -1337,28 +1345,28 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K31" s="3">
         <v>3</v>
@@ -1366,28 +1374,28 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K32" s="3">
         <v>5</v>
@@ -1395,28 +1403,28 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K33" s="3">
         <v>3</v>
@@ -1424,28 +1432,28 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K34" s="3">
         <v>1</v>
@@ -1453,28 +1461,28 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K35" s="3">
         <v>1</v>

</xml_diff>